<commit_message>
repaired. error occurs when double calling get value
</commit_message>
<xml_diff>
--- a/Ttt.xlsx
+++ b/Ttt.xlsx
@@ -10,18 +10,17 @@
         <vt:lpstr>워크시트</vt:lpstr>
       </vt:variant>
       <vt:variant>
-        <vt:i4>6</vt:i4>
+        <vt:i4>5</vt:i4>
       </vt:variant>
     </vt:vector>
   </HeadingPairs>
   <TitlesOfParts>
-    <vt:vector size="6" baseType="lpstr">
+    <vt:vector size="5" baseType="lpstr">
+      <vt:lpstr>Sheet1</vt:lpstr>
       <vt:lpstr>TestSheet1</vt:lpstr>
       <vt:lpstr>TesetSheet2</vt:lpstr>
-      <vt:lpstr>Sheet1</vt:lpstr>
       <vt:lpstr>Sheet2</vt:lpstr>
       <vt:lpstr>Sheet3</vt:lpstr>
-      <vt:lpstr>Asdfa</vt:lpstr>
     </vt:vector>
   </TitlesOfParts>
   <Company/>
@@ -37,7 +36,7 @@
   <dc:creator/>
   <cp:lastModifiedBy/>
   <dcterms:created xsi:type="dcterms:W3CDTF">2006-09-16T00:00:00Z</dcterms:created>
-  <dcterms:modified xsi:type="dcterms:W3CDTF">2021-10-10T09:08:56Z</dcterms:modified>
+  <dcterms:modified xsi:type="dcterms:W3CDTF">2021-10-10T19:59:25Z</dcterms:modified>
 </cp:coreProperties>
 </file>
 
@@ -537,26 +536,40 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="TesetSheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="TestSheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="TesetSheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
-    <sheet name="Asdfa" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl\worksheets\sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl\worksheets\sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -671,7 +684,7 @@
 </worksheet>
 </file>
 
-<file path=xl\worksheets\sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl\worksheets\sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I7"/>
   <sheetViews>
@@ -790,19 +803,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl\worksheets\sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -840,18 +840,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl\worksheets\sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>